<commit_message>
Fix compile error and game balance
</commit_message>
<xml_diff>
--- a/Game Design/GameDesignData.xlsx
+++ b/Game Design/GameDesignData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xwila\Documents\GitHub\TouhouPrideGameJam4\Game Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB9EA0C-418C-4A2F-B4EB-8155D4F3E13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2126DBD-2844-4A26-9476-23E6A6980231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{87B5070D-923F-48C1-B320-26591FEE16EF}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Weapon" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_GameDesignData.xlsxTable1" hidden="1">Table1[]</definedName>
-    <definedName name="_xlcn.WorksheetConnection_GameDesignData.xlsxTable2" hidden="1">Table2[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_GameDesignData.xlsxTable11" hidden="1">Table1[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_GameDesignData.xlsxTable21" hidden="1">Table2[]</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +61,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table1" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_GameDesignData.xlsxTable1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_GameDesignData.xlsxTable11"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -70,7 +70,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table2">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_GameDesignData.xlsxTable2"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_GameDesignData.xlsxTable21"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1"/>
@@ -333,6 +333,10 @@
   </si>
   <si>
     <t>Counter Attack</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Remilia</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -379,11 +383,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="56" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -422,13 +429,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{593CD908-77E8-4F23-92F9-7E21D335B084}" name="Table2" displayName="Table2" ref="Q1:V7" totalsRowShown="0">
-  <autoFilter ref="Q1:V7" xr:uid="{593CD908-77E8-4F23-92F9-7E21D335B084}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{593CD908-77E8-4F23-92F9-7E21D335B084}" name="Table2" displayName="Table2" ref="Q1:V8" totalsRowShown="0">
+  <autoFilter ref="Q1:V8" xr:uid="{593CD908-77E8-4F23-92F9-7E21D335B084}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{DCDA1FD1-7CED-48DE-9B23-49CCB6440831}" name="Name"/>
     <tableColumn id="2" xr3:uid="{2A78288D-DBE4-4FAD-AA93-7B40CB52CB15}" name="Health"/>
     <tableColumn id="3" xr3:uid="{90942DC6-2161-45CE-B3B8-EFAF77DCDE87}" name="Damage" dataDxfId="0">
-      <calculatedColumnFormula>B3</calculatedColumnFormula>
+      <calculatedColumnFormula>B7</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{919A0AA9-3615-47C4-B9C0-8350BD6E396E}" name="Time Bf Att"/>
     <tableColumn id="4" xr3:uid="{0B7046A7-EB49-40DC-B4C6-EC5589948313}" name="Is Alliee"/>
@@ -760,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3E6582-07AC-499E-9E79-114CCA904154}">
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -881,7 +888,7 @@
         <v>20</v>
       </c>
       <c r="S2">
-        <f t="shared" ref="S2:S7" si="0">B3</f>
+        <f t="shared" ref="S2:S8" si="0">B7</f>
         <v>5</v>
       </c>
       <c r="T2">
@@ -937,7 +944,7 @@
       </c>
       <c r="S3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T3">
         <v>1</v>
@@ -992,7 +999,7 @@
       </c>
       <c r="S4">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>10</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -1040,7 +1047,7 @@
       </c>
       <c r="S5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T5">
         <v>1</v>
@@ -1088,7 +1095,7 @@
       </c>
       <c r="S6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-3</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -1130,7 +1137,7 @@
       </c>
       <c r="S7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="T7">
         <v>0</v>
@@ -1157,6 +1164,25 @@
       </c>
       <c r="E8" t="s">
         <v>28</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>66</v>
+      </c>
+      <c r="R8">
+        <v>100</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8" t="s">
+        <v>15</v>
+      </c>
+      <c r="V8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.4">

</xml_diff>